<commit_message>
rendre le site responsive et amélioration de vitesse
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicopatsch/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FF712CA-E2E0-43BA-8DD9-10686C267A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C456495A-AE43-41E0-AECE-C3563D0337B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="620" windowWidth="27860" windowHeight="17380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="620" windowWidth="27860" windowHeight="17380" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
   <si>
     <t>Catégorie</t>
   </si>
@@ -64,7 +65,7 @@
     <t>(SEO ou accessiblité ?)</t>
   </si>
   <si>
-    <t>balise meta title/index</t>
+    <t>balise meta title</t>
   </si>
   <si>
     <t>pas de titre</t>
@@ -154,10 +155,127 @@
     <t>liaison entre les pages</t>
   </si>
   <si>
-    <t>definition d'un langue</t>
+    <t>definition d'une langue</t>
   </si>
   <si>
     <t>site français</t>
+  </si>
+  <si>
+    <t>pas de titre pour le site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mettre des mots clés </t>
+  </si>
+  <si>
+    <t>L5/ index</t>
+  </si>
+  <si>
+    <t>Cacher des mots clés sur le site</t>
+  </si>
+  <si>
+    <t>Eviter les blackhat</t>
+  </si>
+  <si>
+    <t>Supprimer</t>
+  </si>
+  <si>
+    <t>L41/index-L43/index</t>
+  </si>
+  <si>
+    <t>definir des balises alt</t>
+  </si>
+  <si>
+    <t>bien décrire les images</t>
+  </si>
+  <si>
+    <t>Attribut de style dans le html</t>
+  </si>
+  <si>
+    <t>Problème de maintenance</t>
+  </si>
+  <si>
+    <t>attribut dans un css</t>
+  </si>
+  <si>
+    <t>supprimer les attributs dans html</t>
+  </si>
+  <si>
+    <t>Site pas responsive</t>
+  </si>
+  <si>
+    <t>Perte d'informations en fonction taille</t>
+  </si>
+  <si>
+    <t>Adapter le contenu du site</t>
+  </si>
+  <si>
+    <t>Rendre le site responsive</t>
+  </si>
+  <si>
+    <t>Utilisation de balise pagination</t>
+  </si>
+  <si>
+    <t>Pas de lien entre les pages</t>
+  </si>
+  <si>
+    <t>créer un lien entre les pages</t>
+  </si>
+  <si>
+    <t>ajouter pagination next</t>
+  </si>
+  <si>
+    <t>Minifier les fichiers</t>
+  </si>
+  <si>
+    <t>Alourdit nos fichiers</t>
+  </si>
+  <si>
+    <t>compresser nos css et js</t>
+  </si>
+  <si>
+    <t>Images à la place du texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">images plus lourdes que le texte </t>
+  </si>
+  <si>
+    <t>alléger le code pour un site rapide</t>
+  </si>
+  <si>
+    <t>remplacer les images par du texte</t>
+  </si>
+  <si>
+    <t>Liens defectueux</t>
+  </si>
+  <si>
+    <t>Liens cassés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supprimer les liens morts </t>
+  </si>
+  <si>
+    <t>pas de meta robots</t>
+  </si>
+  <si>
+    <t>aucun controle d'inxation</t>
+  </si>
+  <si>
+    <t>ajouter un meta robots</t>
+  </si>
+  <si>
+    <t>definir langue fr</t>
+  </si>
+  <si>
+    <t>Creation des formulaires</t>
+  </si>
+  <si>
+    <t>Pas de type ou mauvaise utlisation</t>
+  </si>
+  <si>
+    <t>definir un type de formulaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">definir le bon type </t>
   </si>
 </sst>
 </file>
@@ -454,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1659,4 +1777,300 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B4BD61-8921-4452-AF63-38A364CBE01E}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="6" max="6" width="31.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
mise a jour du dossier excel
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25525"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25602"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicopatsch/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C456495A-AE43-41E0-AECE-C3563D0337B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA83AB21-846F-474D-85B5-D43BEE8EC0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="620" windowWidth="27860" windowHeight="17380" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="86">
   <si>
     <t>Catégorie</t>
   </si>
@@ -167,9 +167,6 @@
     <t xml:space="preserve">Mettre des mots clés </t>
   </si>
   <si>
-    <t>L5/ index</t>
-  </si>
-  <si>
     <t>Cacher des mots clés sur le site</t>
   </si>
   <si>
@@ -179,7 +176,7 @@
     <t>Supprimer</t>
   </si>
   <si>
-    <t>L41/index-L43/index</t>
+    <t xml:space="preserve">images sans alt ou title </t>
   </si>
   <si>
     <t>definir des balises alt</t>
@@ -188,6 +185,96 @@
     <t>bien décrire les images</t>
   </si>
   <si>
+    <t>Site pas responsive</t>
+  </si>
+  <si>
+    <t>Perte d'informations en fonction taille</t>
+  </si>
+  <si>
+    <t>Adapter le contenu du site</t>
+  </si>
+  <si>
+    <t>Rendre le site responsive</t>
+  </si>
+  <si>
+    <t>Utilisation de balise pagination</t>
+  </si>
+  <si>
+    <t>Pas de lien entre les pages</t>
+  </si>
+  <si>
+    <t>créer un lien entre les pages</t>
+  </si>
+  <si>
+    <t>ajouter pagination next</t>
+  </si>
+  <si>
+    <t>Minifier les fichiers</t>
+  </si>
+  <si>
+    <t>Alourdit nos fichiers</t>
+  </si>
+  <si>
+    <t>compresser nos css,jset images</t>
+  </si>
+  <si>
+    <t>Compresser nos images minifier nos fichiers</t>
+  </si>
+  <si>
+    <t>Allégez les pages de votre site - Optimisez le référencement de votre site (SEO) en améliorant ses performances techniques - OpenClassrooms</t>
+  </si>
+  <si>
+    <t>Images à la place du texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">images plus lourdes que le texte </t>
+  </si>
+  <si>
+    <t>alléger le code pour un site rapide</t>
+  </si>
+  <si>
+    <t>remplacer les images par du texte</t>
+  </si>
+  <si>
+    <t>Liens defectueux</t>
+  </si>
+  <si>
+    <t>Liens cassés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supprimer les liens morts </t>
+  </si>
+  <si>
+    <t>pas de meta robots</t>
+  </si>
+  <si>
+    <t>aucun controle d'inxation</t>
+  </si>
+  <si>
+    <t>ajouter un meta robots</t>
+  </si>
+  <si>
+    <t>definir langue fr</t>
+  </si>
+  <si>
+    <t>Creation des formulaires</t>
+  </si>
+  <si>
+    <t>Pas de type ou mauvaise utlisation</t>
+  </si>
+  <si>
+    <t>definir un type de formulaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">definir le bon type </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Techniques de cloaking </t>
+  </si>
+  <si>
+    <t>Servir un contenu différent aux moteurs de recherche et utilisateurs</t>
+  </si>
+  <si>
     <t>Attribut de style dans le html</t>
   </si>
   <si>
@@ -200,89 +287,26 @@
     <t>supprimer les attributs dans html</t>
   </si>
   <si>
-    <t>Site pas responsive</t>
-  </si>
-  <si>
-    <t>Perte d'informations en fonction taille</t>
-  </si>
-  <si>
-    <t>Adapter le contenu du site</t>
-  </si>
-  <si>
-    <t>Rendre le site responsive</t>
-  </si>
-  <si>
-    <t>Utilisation de balise pagination</t>
-  </si>
-  <si>
-    <t>Pas de lien entre les pages</t>
-  </si>
-  <si>
-    <t>créer un lien entre les pages</t>
-  </si>
-  <si>
-    <t>ajouter pagination next</t>
-  </si>
-  <si>
-    <t>Minifier les fichiers</t>
-  </si>
-  <si>
-    <t>Alourdit nos fichiers</t>
-  </si>
-  <si>
-    <t>compresser nos css et js</t>
-  </si>
-  <si>
-    <t>Images à la place du texte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">images plus lourdes que le texte </t>
-  </si>
-  <si>
-    <t>alléger le code pour un site rapide</t>
-  </si>
-  <si>
-    <t>remplacer les images par du texte</t>
-  </si>
-  <si>
-    <t>Liens defectueux</t>
-  </si>
-  <si>
-    <t>Liens cassés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supprimer les liens morts </t>
-  </si>
-  <si>
-    <t>pas de meta robots</t>
-  </si>
-  <si>
-    <t>aucun controle d'inxation</t>
-  </si>
-  <si>
-    <t>ajouter un meta robots</t>
-  </si>
-  <si>
-    <t>definir langue fr</t>
-  </si>
-  <si>
-    <t>Creation des formulaires</t>
-  </si>
-  <si>
-    <t>Pas de type ou mauvaise utlisation</t>
-  </si>
-  <si>
-    <t>definir un type de formulaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">definir le bon type </t>
+    <t>Aucun découpage de notre code html</t>
+  </si>
+  <si>
+    <t>Aucune maquette et information</t>
+  </si>
+  <si>
+    <t>définir des maquettes et les annoter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">découper notre html en maquette </t>
+  </si>
+  <si>
+    <t>Annotez vos maquettes à l'aide d'informations d'accessibilité - Concevez un contenu web accessible - OpenClassrooms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -312,6 +336,16 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -344,10 +378,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -355,8 +390,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1781,7 +1819,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B4BD61-8921-4452-AF63-38A364CBE01E}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -1819,7 +1857,7 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="15.75">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
@@ -1833,9 +1871,6 @@
       </c>
       <c r="E2" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75">
@@ -1854,9 +1889,6 @@
       <c r="E3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="4" spans="1:7" ht="15.75">
       <c r="A4" t="s">
@@ -1872,9 +1904,6 @@
         <v>40</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="5" spans="1:7" ht="15.75">
       <c r="A5" t="s">
@@ -1884,16 +1913,13 @@
         <v>35</v>
       </c>
       <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
         <v>42</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75">
@@ -1901,16 +1927,16 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
         <v>27</v>
       </c>
       <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75">
@@ -1918,36 +1944,33 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
         <v>48</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>49</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
         <v>52</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>53</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75">
@@ -1955,15 +1978,18 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
         <v>56</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>57</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="6" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1972,22 +1998,30 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="4"/>
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="15.75">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -1996,81 +2030,101 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>66</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="15.75">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:7">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75">
       <c r="A16" t="s">
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F9" r:id="rId1" xr:uid="{F930E537-B16A-41E5-B507-2C82D05A3E6F}"/>
+    <hyperlink ref="F17" r:id="rId2" xr:uid="{D0C7C410-65D9-4930-A725-732EAED96F9E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>